<commit_message>
Tabular Loop generation works #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderLoopDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderLoopDef.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720E68D9-4D3E-4A41-9F56-CAB94F52BC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{730946F5-8BAD-4CAC-863D-60D44A58484F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1005" windowWidth="16800" windowHeight="10155" activeTab="1" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" activeTab="1" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestItem_SeqWithLoop" sheetId="2" r:id="rId1"/>
-    <sheet name="TestItem_StartWithLoop" sheetId="3" r:id="rId2"/>
+    <sheet name="StartWithLoop" sheetId="3" r:id="rId1"/>
+    <sheet name="SequenceWithLoop" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:L30"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -94,9 +90,6 @@
     <t>TestItem_Last:0</t>
   </si>
   <si>
-    <t>Loop</t>
-  </si>
-  <si>
     <t>TestItem_Loop:0</t>
   </si>
   <si>
@@ -113,6 +106,9 @@
   </si>
   <si>
     <t>Loopy</t>
+  </si>
+  <si>
+    <t>Looping</t>
   </si>
 </sst>
 </file>
@@ -256,7 +252,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -265,13 +267,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,27 +583,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB994CB5-5202-4AA9-9615-3F210D52ADE5}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC2A13-BBF2-4C2B-ADB3-E20C68234B9A}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -616,15 +612,15 @@
       <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -653,98 +649,50 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -757,44 +705,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC2A13-BBF2-4C2B-ADB3-E20C68234B9A}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB994CB5-5202-4AA9-9615-3F210D52ADE5}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -823,50 +771,98 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Tabular Nested Loop generation works #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderLoopDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderLoopDef.xlsx
@@ -3,16 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{730946F5-8BAD-4CAC-863D-60D44A58484F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C668AD8C-8E93-4AC9-9068-F86EFCD588E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" activeTab="1" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="1890" yWindow="920" windowWidth="16800" windowHeight="10160" activeTab="2" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="StartWithLoop" sheetId="3" r:id="rId1"/>
     <sheet name="SequenceWithLoop" sheetId="2" r:id="rId2"/>
+    <sheet name="LoopContainLoop" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L30"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Description</t>
   </si>
@@ -587,7 +592,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB994CB5-5202-4AA9-9615-3F210D52ADE5}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -872,4 +877,154 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA06548-09BC-49A3-B20B-D97431A5E720}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Loop properties (RoutingExpr) works #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderLoopDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderLoopDef.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C668AD8C-8E93-4AC9-9068-F86EFCD588E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54AB8C5-363C-4C65-ACDA-460C61A455B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="920" windowWidth="16800" windowHeight="10160" activeTab="2" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="3585" yWindow="1200" windowWidth="19470" windowHeight="11235" tabRatio="625" firstSheet="1" activeTab="5" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
-    <sheet name="StartWithLoop" sheetId="3" r:id="rId1"/>
-    <sheet name="SequenceWithLoop" sheetId="2" r:id="rId2"/>
-    <sheet name="LoopContainLoop" sheetId="4" r:id="rId3"/>
+    <sheet name="Template" sheetId="5" r:id="rId1"/>
+    <sheet name="StartWithLoop" sheetId="3" r:id="rId2"/>
+    <sheet name="StartWithLoopInfinite" sheetId="6" r:id="rId3"/>
+    <sheet name="SequenceWithLoop" sheetId="2" r:id="rId4"/>
+    <sheet name="NestedLoops" sheetId="4" r:id="rId5"/>
+    <sheet name="LoopProperties" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -114,6 +117,15 @@
   </si>
   <si>
     <t>Looping</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>RoutingScript</t>
   </si>
 </sst>
 </file>
@@ -588,27 +600,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC2A13-BBF2-4C2B-ADB3-E20C68234B9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C2E7B4-2BDE-4184-BF63-F0DDBF13D7E1}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -625,7 +637,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -654,9 +666,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -669,7 +681,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -686,7 +698,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -710,27 +722,159 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC2A13-BBF2-4C2B-ADB3-E20C68234B9A}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082DF1A3-7243-47C1-8BE3-F4CC9AC0A27E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB994CB5-5202-4AA9-9615-3F210D52ADE5}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -747,7 +891,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -776,7 +920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -799,7 +943,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -814,7 +958,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -833,7 +977,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -846,7 +990,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -879,45 +1023,115 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA06548-09BC-49A3-B20B-D97431A5E720}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EFAFEC-EF60-49F0-AD68-A06BDF79223B}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -928,102 +1142,49 @@
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>